<commit_message>
added objects for trials
</commit_message>
<xml_diff>
--- a/OutputFiles/TC01_Trials_Filter_Diagnosis-AdenoCervix_Neo4jData.xlsx
+++ b/OutputFiles/TC01_Trials_Filter_Diagnosis-AdenoCervix_Neo4jData.xlsx
@@ -10,12 +10,14 @@
     <sheet name="CypherOutput_Message" r:id="rId4" sheetId="2"/>
     <sheet name="StatOuput" r:id="rId5" sheetId="3"/>
     <sheet name="StatOuput_Message" r:id="rId6" sheetId="4"/>
+    <sheet name="CaseDetailStat" r:id="rId7" sheetId="5"/>
+    <sheet name="CaseDetailStat_Message" r:id="rId8" sheetId="6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="33">
   <si>
     <t>Case ID</t>
   </si>
@@ -108,6 +110,12 @@
   </si>
   <si>
     <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report) WITH DISTINCT c AS c, t ,a, s WHERE c.disease IN ['Adenocarcinoma of the cervix'] OPTIONAL MATCH (s)&lt;-[*]-(f:file) RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(t.clinical_trial_designation)) as number_of_trial</t>
+  </si>
+  <si>
+    <t>Cypher query should not be an empty string</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -424,4 +432,186 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>